<commit_message>
update with csv files
</commit_message>
<xml_diff>
--- a/eta analysis.xlsx
+++ b/eta analysis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jmonkeyp\ETA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D66CA7D0-3F76-48E5-961D-E30DAFA6FDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8F53C4-1623-484F-BF2C-8B23EE60B402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="segments 0.5 1.0i" sheetId="1" r:id="rId1"/>
     <sheet name="segments 0.5 1.5i" sheetId="2" r:id="rId2"/>
     <sheet name="main" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>segment</t>
   </si>
@@ -41,11 +52,20 @@
   <si>
     <t>anglediff</t>
   </si>
+  <si>
+    <t>ln(segmentnumber) * 28.6478897565417</t>
+  </si>
+  <si>
+    <t>formula?=</t>
+  </si>
+  <si>
+    <t>ln(segmentnumber) * constant factor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2186,7 +2206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4734,7 +4754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7282,11 +7302,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M150"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7866,7 +7886,7 @@
         <v>77.579923616354961</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7902,7 +7922,7 @@
         <v>79.428816054955007</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7938,7 +7958,7 @@
         <v>81.165583537283965</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7974,7 +7994,7 @@
         <v>82.80305147562899</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8010,7 +8030,7 @@
         <v>84.35196327002302</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8046,7 +8066,7 @@
         <v>85.821407912887025</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8082,7 +8102,7 @@
         <v>87.21914315721699</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8118,7 +8138,7 @@
         <v>88.551843436598006</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8154,7 +8174,7 @@
         <v>89.825292630210015</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8190,7 +8210,7 @@
         <v>91.044535772162021</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8226,7 +8246,7 @@
         <v>92.213999770819044</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8261,8 +8281,14 @@
         <f t="shared" si="0"/>
         <v>93.337590437408039</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P27" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -8297,8 +8323,14 @@
         <f t="shared" si="0"/>
         <v>94.418771192836005</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P28" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -8334,7 +8366,7 @@
         <v>95.460627453747975</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -8370,7 +8402,7 @@
         <v>96.465919715114012</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -8406,7 +8438,7 @@
         <v>97.437127630093983</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>